<commit_message>
GE, JU, OW, VD
</commit_message>
<xml_diff>
--- a/GE_VEGETATION_einheiten_unique_bh2025_mf_bh.xlsx
+++ b/GE_VEGETATION_einheiten_unique_bh2025_mf_bh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\develops\sensitivewaldstandorteCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9EF1F8-B7BC-4371-AA98-F596EF872536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F09B55-4C2F-4BAD-A3AA-94E8563F60D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42795" yWindow="2280" windowWidth="19215" windowHeight="19875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47085" yWindow="2115" windowWidth="27915" windowHeight="19530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1064,15 +1064,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="61.140625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="8" width="20" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>